<commit_message>
ver excel celdas en amarillo
</commit_message>
<xml_diff>
--- a/Planilla de carga.xlsx
+++ b/Planilla de carga.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <r>
       <t>titulo:[</t>
@@ -765,9 +765,6 @@
     <t>otro parrafo</t>
   </si>
   <si>
-    <t>arreglar con ESBLANCO</t>
-  </si>
-  <si>
     <t>{titulo:[</t>
   </si>
   <si>
@@ -783,12 +780,6 @@
     <t>ewrwer</t>
   </si>
   <si>
-    <t>ert</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
     <t>parrafo medio grande oe</t>
   </si>
   <si>
@@ -805,13 +796,28 @@
   </si>
   <si>
     <t>2/  p</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>aquí</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +854,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -856,7 +869,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -881,8 +894,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -890,11 +909,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -915,7 +949,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1220,38 +1269,40 @@
   <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="6" width="7.28515625" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" customWidth="1"/>
-    <col min="8" max="12" width="5.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="11" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" customWidth="1"/>
     <col min="13" max="13" width="16.140625" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" customWidth="1"/>
-    <col min="15" max="15" width="54.5703125" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="M1" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
@@ -1287,232 +1338,250 @@
       <c r="L2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="4" t="str">
-        <f>+IF(ISBLANK($E2),
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="14" t="str">
+        <f t="shared" ref="M3:M8" si="0">+IF(ISBLANK($E2),
             IF(ISBLANK(B3),
-                       "",M$2&amp;""""&amp;$B3&amp;"""],"  ),
+                        IF(ISBLANK(C3),
+                                 "-----",M$2&amp;"null],"),
+                        M$2&amp;""""&amp;B3&amp;"""],"  ),
              IF(ISBLANK(B3),
-                       M$2&amp;"null],",M$2&amp;""""&amp;$B3&amp;"""],"  ))</f>
+                       M$2&amp;"null],",M$2&amp;""""&amp;B3&amp;"""],"  ))</f>
         <v>{titulo:["wer"],</v>
       </c>
-      <c r="N3" s="4" t="str">
-        <f>+IF(ISBLANK($E2),
+      <c r="N3" s="14" t="str">
+        <f t="shared" ref="N3:N6" si="1">+IF(ISBLANK($E2),
             IF(ISBLANK(C3),
-                       "",N$2&amp;""""&amp;$B3&amp;"""],"  ),
+                       IF(ISBLANK(B3),"-----",N$2&amp;"null],"),
+                        N$2&amp;""""&amp;C3&amp;"""],"  ),
              IF(ISBLANK(C3),
-                       N$2&amp;"null],",N$2&amp;""""&amp;$B3&amp;"""],"  ))</f>
-        <v>subtitulo:["wer"],</v>
-      </c>
-      <c r="O3" s="4" t="str">
-        <f t="shared" ref="O3:O4" si="0">IF(ISBLANK(D3),O$2&amp;"null],",
+                       N$2&amp;"null],",N$2&amp;""""&amp;C3&amp;"""],"  ))</f>
+        <v>subtitulo:[null],</v>
+      </c>
+      <c r="O3" s="14" t="str">
+        <f t="shared" ref="O3:O4" si="2">IF(ISBLANK(D3),O$2&amp;"null],",
      IF(ISBLANK(E2),
           IF(ISBLANK(E3),""""&amp;D3&amp;""",",""""&amp;D3&amp;"""],"),
                 IF(ISBLANK(E3),O$2&amp;""""&amp;D3&amp;""",",O$2&amp;""""&amp;D3&amp;"""],")))</f>
-        <v>parrafo:["el parrafo en cuestión"],</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>parrafo:["el parrafo en cuestión",</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="4" t="str">
-        <f>+IF(ISBLANK($E3),
-            IF(ISBLANK(B4),
-                       "",M$2&amp;""""&amp;$B4&amp;"""],"  ),
-             IF(ISBLANK(B4),
-                       M$2&amp;"null],",M$2&amp;""""&amp;$B4&amp;"""],"  ))</f>
-        <v>{titulo:[null],</v>
-      </c>
-      <c r="N4" s="4" t="str">
-        <f t="shared" ref="N4:N8" si="1">+IF(ISBLANK($E3),
-            IF(ISBLANK(C4),
-                       "",N$2&amp;""""&amp;$B4&amp;"""],"  ),
-             IF(ISBLANK(C4),
-                       N$2&amp;"null],",N$2&amp;""""&amp;$B4&amp;"""],"  ))</f>
-        <v>subtitulo:[null],</v>
-      </c>
-      <c r="O4" s="4" t="str">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>parrafo:["otro parrafo",</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>-----</v>
+      </c>
+      <c r="N4" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>-----</v>
+      </c>
+      <c r="O4" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>"otro parrafo",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="4" t="str">
-        <f t="shared" ref="M5:M8" si="2">+IF(ISBLANK($E4),
-            IF(ISBLANK(B5),
-                       "",M$2&amp;""""&amp;$B5&amp;"""],"  ),
-             IF(ISBLANK(B5),
-                       M$2&amp;"null],",M$2&amp;""""&amp;$B5&amp;"""],"  ))</f>
-        <v/>
-      </c>
-      <c r="N5" s="4" t="str">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>-----</v>
+      </c>
+      <c r="N5" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O5" s="4" t="str">
+        <v>-----</v>
+      </c>
+      <c r="O5" s="14" t="str">
         <f>IF(ISBLANK(D5),O$2&amp;"null],",
      IF(ISBLANK(E4),
           IF(ISBLANK(E5),""""&amp;D5&amp;""",",""""&amp;D5&amp;"""],"),
                 IF(ISBLANK(E5),O$2&amp;""""&amp;D5&amp;""",",O$2&amp;""""&amp;D5&amp;"""],")))</f>
-        <v>"ewrwer",</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>"ewrwer"],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N6" s="4" t="str">
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>{titulo:["sdf"],</v>
+      </c>
+      <c r="N6" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O6" s="4" t="str">
+        <v>subtitulo:[null],</v>
+      </c>
+      <c r="O6" s="15" t="str">
         <f>IF(ISBLANK(D6),O$2&amp;"null],",
      IF(ISBLANK(E5),
-          IF(ISBLANK(E6),""""&amp;D6&amp;""",",""""&amp;D6&amp;"""],"),
+          IF(ISBLANK(E6),""""&amp;D6&amp;""",",
+                                                                             IF(AND(ISBLANK(B6),ISBLANK(C6)),O$2&amp;""""&amp;D6&amp;"""],",""""&amp;D6&amp;"""],")),
                 IF(ISBLANK(E6),O$2&amp;""""&amp;D6&amp;""",",O$2&amp;""""&amp;D6&amp;"""],")))</f>
-        <v>"parrafo medio grande oe"],</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>parrafo:["parrafo medio grande oe",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="I7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="4" t="str">
-        <f t="shared" si="2"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>-----</v>
+      </c>
+      <c r="N7" s="14" t="str">
+        <f>+IF(ISBLANK($E6),
+            IF(ISBLANK(C7),
+                       IF(ISBLANK(B7),"-----",N$2&amp;"null],"),
+                        N$2&amp;""""&amp;C7&amp;"""],"  ),
+             IF(ISBLANK(C7),
+                       N$2&amp;"null],",N$2&amp;""""&amp;C7&amp;"""],"  ))</f>
+        <v>-----</v>
+      </c>
+      <c r="O7" s="15" t="str">
+        <f>IF(ISBLANK(D7),O$2&amp;"null],",
+     IF(ISBLANK(E6),
+          IF(ISBLANK(E7),
+                                               """"&amp;D7&amp;""",",
+                                               IF(OR(ISBLANK(B7),ISBLANK(C7)),""""&amp;D7&amp;"""],",O$2&amp;""""&amp;D7&amp;"""],")),
+                IF(ISBLANK(E7),O$2&amp;""""&amp;D7&amp;""",",O$2&amp;""""&amp;D7&amp;"""],")))</f>
+        <v>"aquí"],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10">
+        <v>45</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="14" t="str">
+        <f t="shared" si="0"/>
         <v>{titulo:[null],</v>
       </c>
-      <c r="N7" s="4" t="str">
-        <f t="shared" si="1"/>
+      <c r="N8" s="16" t="str">
+        <f>+IF(ISBLANK($E7),
+            IF(ISBLANK(C8),
+                       IF(ISBLANK(B8),"-----",N$2&amp;"null],"),
+                        N$2&amp;""""&amp;C8&amp;"""],"  ),
+             IF(ISBLANK(C8),
+                       N$2&amp;"null],",N$2&amp;""""&amp;C8&amp;"""],"  ))</f>
         <v>subtitulo:[null],</v>
       </c>
-      <c r="O7" s="4" t="str">
-        <f t="shared" ref="O7:O8" si="3">IF(ISBLANK(D7),O$2&amp;"null],",
-     IF(ISBLANK(E6),
-          IF(ISBLANK(E7),""""&amp;D7&amp;""",",""""&amp;D7&amp;"""],"),
-                IF(ISBLANK(E7),O$2&amp;""""&amp;D7&amp;""",",O$2&amp;""""&amp;D7&amp;"""],")))</f>
-        <v>parrafo:["asdf",</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="O8" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>parrafo:[null],</v>
+      <c r="O8" s="14" t="str">
+        <f t="shared" ref="O8" si="3">IF(ISBLANK(D8),O$2&amp;"null],",
+     IF(ISBLANK(E7),
+          IF(ISBLANK(E8),""""&amp;D8&amp;""",",
+                                                                             IF(AND(ISBLANK(B8),ISBLANK(C8)),O$2&amp;""""&amp;D8&amp;"""],",""""&amp;D8&amp;"""],")),
+                IF(ISBLANK(E8),O$2&amp;""""&amp;D8&amp;""",",O$2&amp;""""&amp;D8&amp;"""],")))</f>
+        <v>parrafo:["45",</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1520,16 +1589,45 @@
       <c r="K9" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M11" s="10"/>
+      <c r="M11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O11" s="8" t="str">
+        <f t="shared" ref="O11" si="4">+IF(OR(ISBLANK(M11),ISBLANK(N11)),"es","nuez")</f>
+        <v>es</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O12" s="17" t="str">
+        <f>+IF(OR(ISBLANK(M12),ISBLANK(N12)),"es","nuez")</f>
+        <v>es</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="M13" t="s">
+        <v>62</v>
+      </c>
+      <c r="N13" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" ref="O13:O14" si="5">+IF(OR(ISBLANK(M13),ISBLANK(N13)),"es","nuez")</f>
+        <v>nuez</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="5"/>
+        <v>es</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>